<commit_message>
Extract axls generartor from controller to lib
</commit_message>
<xml_diff>
--- a/public/xlsx/participants.xlsx
+++ b/public/xlsx/participants.xlsx
@@ -89,39 +89,40 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.2561797752809"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.28988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0561797752809"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.656179775280899"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.2561797752809"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.28988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.0561797752809"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.8561797752809"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="42.8561797752809"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.4561797752809"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="23.0561797752809"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.0561797752809"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.18988764044944"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.8561797752809"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="42.8561797752809"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.4561797752809"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="23.0561797752809"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="28.4561797752809"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.4561797752809"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="26.6561797752809"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="8.656179775280899"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.0561797752809"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.2561797752809"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="14.0561797752809"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.4561797752809"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="183.48988764044947"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="10.4561797752809"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.0561797752809"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="21.2561797752809"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="33.8561797752809"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.4561797752809"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.0561797752809"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="30.2561797752809"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="21.2561797752809"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.0561797752809"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="28.4561797752809"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.4561797752809"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="26.6561797752809"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.656179775280899"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0561797752809"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.2561797752809"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="14.0561797752809"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="10.4561797752809"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="183.48988764044947"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.4561797752809"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="23.0561797752809"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="21.2561797752809"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="33.8561797752809"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="10.4561797752809"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="23.0561797752809"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="30.2561797752809"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="21.2561797752809"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -135,135 +136,140 @@
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
+          <t>No.</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
           <t>Registro</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>Fecha de registro</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="D3" s="4" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>Apellidos</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="F3" s="4" t="inlineStr">
         <is>
           <t>Correo</t>
         </is>
       </c>
-      <c r="F3" s="4" t="inlineStr">
+      <c r="G3" s="4" t="inlineStr">
         <is>
           <t>Teléfono(s)</t>
         </is>
       </c>
-      <c r="G3" s="4" t="inlineStr">
+      <c r="H3" s="4" t="inlineStr">
         <is>
           <t>Institución empresa en donde labora</t>
         </is>
       </c>
-      <c r="H3" s="4" t="inlineStr">
+      <c r="I3" s="4" t="inlineStr">
         <is>
           <t>Costo</t>
         </is>
       </c>
-      <c r="I3" s="4" t="inlineStr">
+      <c r="J3" s="4" t="inlineStr">
         <is>
           <t>Titulo de licenciatura</t>
         </is>
       </c>
-      <c r="J3" s="4" t="inlineStr">
+      <c r="K3" s="4" t="inlineStr">
         <is>
           <t>Titulo de Maestría</t>
         </is>
       </c>
-      <c r="K3" s="4" t="inlineStr">
+      <c r="L3" s="4" t="inlineStr">
         <is>
           <t>Título de Doctorado</t>
         </is>
       </c>
-      <c r="L3" s="4" t="inlineStr">
+      <c r="M3" s="4" t="inlineStr">
         <is>
           <t>Requiere factura</t>
         </is>
       </c>
-      <c r="M3" s="4" t="inlineStr">
+      <c r="N3" s="4" t="inlineStr">
         <is>
           <t>Nombre o razón social</t>
         </is>
       </c>
-      <c r="N3" s="4" t="inlineStr">
+      <c r="O3" s="4" t="inlineStr">
         <is>
           <t>RFC</t>
         </is>
       </c>
-      <c r="O3" s="4" t="inlineStr">
+      <c r="P3" s="4" t="inlineStr">
         <is>
           <t>Dirección Fiscal</t>
         </is>
       </c>
-      <c r="P3" s="4" t="inlineStr">
+      <c r="Q3" s="4" t="inlineStr">
         <is>
           <t>Ciudad</t>
         </is>
       </c>
-      <c r="Q3" s="4" t="inlineStr">
+      <c r="R3" s="4" t="inlineStr">
         <is>
           <t>Municipio</t>
         </is>
       </c>
-      <c r="R3" s="4" t="inlineStr">
+      <c r="S3" s="4" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
       </c>
-      <c r="S3" s="4" t="inlineStr">
+      <c r="T3" s="4" t="inlineStr">
         <is>
           <t>Razones por la que desea asisitir al curso</t>
         </is>
       </c>
-      <c r="T3" s="4" t="inlineStr">
+      <c r="U3" s="4" t="inlineStr">
         <is>
           <t>Edad</t>
         </is>
       </c>
-      <c r="U3" s="4" t="inlineStr">
+      <c r="V3" s="4" t="inlineStr">
         <is>
           <t>Tipo de sangre</t>
         </is>
       </c>
-      <c r="V3" s="4" t="inlineStr">
+      <c r="W3" s="4" t="inlineStr">
         <is>
           <t>Traera computadora</t>
         </is>
       </c>
-      <c r="W3" s="4" t="inlineStr">
+      <c r="X3" s="4" t="inlineStr">
         <is>
           <t>Ya ha tomado el curso antes</t>
         </is>
       </c>
-      <c r="X3" s="4" t="inlineStr">
+      <c r="Y3" s="4" t="inlineStr">
         <is>
           <t>Idioma</t>
         </is>
       </c>
-      <c r="Y3" s="4" t="inlineStr">
+      <c r="Z3" s="4" t="inlineStr">
         <is>
           <t>Ficha de depósito</t>
         </is>
       </c>
-      <c r="Z3" s="4" t="inlineStr">
+      <c r="AA3" s="4" t="inlineStr">
         <is>
           <t>Carte de recomendación</t>
         </is>
       </c>
-      <c r="AA3" s="4" t="inlineStr">
+      <c r="AB3" s="4" t="inlineStr">
         <is>
           <t>Carta de motivos</t>
         </is>
@@ -271,42 +277,40 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="2">
         <v>41858.34250753924</v>
       </c>
-      <c r="C4" s="0" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>Ramón</t>
         </is>
       </c>
-      <c r="D4" s="0" t="inlineStr">
+      <c r="E4" s="0" t="inlineStr">
         <is>
           <t>Martínez Olvera</t>
         </is>
       </c>
-      <c r="E4" s="0" t="inlineStr">
+      <c r="F4" s="0" t="inlineStr">
         <is>
           <t>martinezo@inb.unam.mx</t>
         </is>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>2381052</v>
       </c>
-      <c r="G4" s="0" t="inlineStr">
+      <c r="H4" s="0" t="inlineStr">
         <is>
           <t>INB-UNAM</t>
         </is>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>1500.0</v>
       </c>
-      <c r="I4" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
       <c r="J4" s="0" t="inlineStr">
         <is>
           <t/>
@@ -317,14 +321,14 @@
           <t/>
         </is>
       </c>
-      <c r="L4" s="0" t="b">
+      <c r="L4" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M4" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="M4" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
       <c r="N4" s="0" t="inlineStr">
         <is>
           <t/>
@@ -347,44 +351,49 @@
       </c>
       <c r="R4" s="0" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S4" s="0" t="inlineStr">
+        <is>
           <t>Campeche</t>
         </is>
       </c>
-      <c r="S4" s="0" t="inlineStr">
+      <c r="T4" s="0" t="inlineStr">
         <is>
           <t>smdsa jasdlk ajs akjd lkja añlfm sd. wdnmdsm, sjfnjksd sdfjk snbsd sdjfb sdbfjk lsdhflkjsdf lksmdsa jasdlk ajs akjd lkja añlfm sd. wdnmdsm, sjfnjksd sdfjk snbsd sdjfb sdbfjk lsdhflkjsdf lksmdsa jasdlk ajs akjd lkja añlfm sd. wdnmdsm, sjfnjksd sdfjk snbsd sdjfb sdbfjk lsdhflkjsdf lksmdsa jasdlk ajs akjd lkja añlfm sd. wdnmdsm, sjfnjksd sdfjk snbsd sdjfb sdbfjk lsdhflkjsdf lk</t>
         </is>
       </c>
-      <c r="T4" s="0" t="n">
+      <c r="U4" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="U4" s="0" t="inlineStr">
+      <c r="V4" s="0" t="inlineStr">
         <is>
           <t>B+</t>
         </is>
       </c>
-      <c r="V4" s="0" t="b">
+      <c r="W4" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="W4" s="0" t="b">
+      <c r="X4" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="X4" s="0" t="inlineStr">
+      <c r="Y4" s="0" t="inlineStr">
         <is>
           <t> Español</t>
         </is>
       </c>
-      <c r="Y4" s="0" t="inlineStr">
+      <c r="Z4" s="0" t="inlineStr">
         <is>
           <t>daniela_sticker.psd</t>
         </is>
       </c>
-      <c r="Z4" s="0" t="inlineStr">
+      <c r="AA4" s="0" t="inlineStr">
         <is>
           <t>emiliano_stickers.psd</t>
         </is>
       </c>
-      <c r="AA4" s="0" t="inlineStr">
+      <c r="AB4" s="0" t="inlineStr">
         <is>
           <t>david_sticker.psd</t>
         </is>

</xml_diff>